<commit_message>
fix example excel files
</commit_message>
<xml_diff>
--- a/docs/assets/files/AuthorArranger Example.xlsx
+++ b/docs/assets/files/AuthorArranger Example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projects\nci-webtools-dceg-author-arranger\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\nci-webtools-dceg-author-arranger\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5490B047-846C-4824-B782-A5E66FAABEA1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
-    <sheet name="Template" sheetId="2" r:id="rId2"/>
+    <sheet name="Authors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -144,16 +145,16 @@
     <t>MS</t>
   </si>
   <si>
-    <t>Center for Biomedical Informatics and Information Technology, National Cancer Institude, Rockville, MD, USA</t>
-  </si>
-  <si>
     <t>Office of the Directory, Division of Cancer Epidemiology and Genetics, National Cancer Institute, Rockville, MD, USA</t>
+  </si>
+  <si>
+    <t>Center for Biomedical Informatics and Information Technology, National Cancer Institute, Rockville, MD, USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,7 +517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -636,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +707,7 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -723,7 +724,7 @@
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>